<commit_message>
(#22)Updated testdata for Recommended Content
</commit_message>
<xml_diff>
--- a/test-data/recommendedcontent-data.xlsx
+++ b/test-data/recommendedcontent-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cgov_workspace\cgov-digital-platform-qa\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E151A508-683E-46E1-A4DF-9F221FA49F98}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EEA90D0-C9B9-48B9-871A-AB08A257627E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{112BCE41-1B7B-AF44-BEF2-07A92CFC037C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="15820" xr2:uid="{112BCE41-1B7B-AF44-BEF2-07A92CFC037C}"/>
   </bookViews>
   <sheets>
     <sheet name="pages_with_recommended_content" sheetId="9" r:id="rId1"/>
@@ -88,9 +88,6 @@
     <t>pet_mm_featured.jpg</t>
   </si>
   <si>
-    <t>/sites/default/files/styles/cgov_featured/public/cgov_image/featured/2019-11/</t>
-  </si>
-  <si>
     <t>find-clinical-trial-blue-feature-card-feat.jpg</t>
   </si>
   <si>
@@ -122,6 +119,9 @@
   </si>
   <si>
     <t>externalCardIndex</t>
+  </si>
+  <si>
+    <t>/sites/default/files/styles/cgov_featured/public/cgov_image/featured/</t>
   </si>
 </sst>
 </file>
@@ -490,26 +490,26 @@
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
-    <col min="3" max="4" width="9.875" customWidth="1"/>
+    <col min="3" max="4" width="9.83203125" customWidth="1"/>
     <col min="5" max="5" width="12.5" customWidth="1"/>
-    <col min="6" max="6" width="9.875" customWidth="1"/>
-    <col min="7" max="8" width="15.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.625" customWidth="1"/>
+    <col min="6" max="6" width="9.83203125" customWidth="1"/>
+    <col min="7" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.58203125" customWidth="1"/>
     <col min="10" max="10" width="67.75" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="36.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="36.58203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="47.25" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -523,16 +523,16 @@
         <v>16</v>
       </c>
       <c r="E1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F1" t="s">
         <v>6</v>
       </c>
       <c r="G1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" t="s">
         <v>30</v>
-      </c>
-      <c r="H1" t="s">
-        <v>31</v>
       </c>
       <c r="I1" t="s">
         <v>9</v>
@@ -541,10 +541,10 @@
         <v>12</v>
       </c>
       <c r="K1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" t="s">
         <v>24</v>
-      </c>
-      <c r="L1" t="s">
-        <v>25</v>
       </c>
       <c r="M1" t="s">
         <v>13</v>
@@ -556,7 +556,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -570,7 +570,7 @@
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -582,19 +582,19 @@
         <v>7</v>
       </c>
       <c r="J2" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="K2" t="s">
         <v>19</v>
       </c>
       <c r="L2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -608,7 +608,7 @@
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -620,19 +620,19 @@
         <v>7</v>
       </c>
       <c r="J3" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="K3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" t="s">
         <v>26</v>
-      </c>
-      <c r="L3" t="s">
-        <v>27</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="31" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -655,13 +655,13 @@
         <v>8</v>
       </c>
       <c r="J4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" t="s">
         <v>20</v>
       </c>
-      <c r="K4" t="s">
-        <v>21</v>
-      </c>
       <c r="L4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>11</v>
@@ -684,13 +684,13 @@
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="71.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="71.08203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -698,7 +698,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>

</xml_diff>